<commit_message>
Updated to reflect current status
</commit_message>
<xml_diff>
--- a/Si5351_register_map.xlsx
+++ b/Si5351_register_map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\SI5351 library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\SI5351 library\si5351EasyLib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B99DC1-D138-4D69-819E-643DE3417FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A4AB09-2705-4EFE-9A3D-F84A37B083C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="696" yWindow="0" windowWidth="11820" windowHeight="12360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1671,55 +1671,28 @@
     <xf numFmtId="166" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1728,7 +1701,34 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2061,11 +2061,11 @@
       <c r="E6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="41" t="s">
+      <c r="H6" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
     </row>
     <row r="8" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
@@ -2130,10 +2130,10 @@
       <c r="J10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="42" t="s">
+      <c r="K10" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="L10" s="42"/>
+      <c r="L10" s="59"/>
       <c r="M10" s="12"/>
     </row>
     <row r="11" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -2201,11 +2201,11 @@
       <c r="I15" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="J15" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="K15" s="43"/>
-      <c r="L15" s="43"/>
+      <c r="J15" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="55"/>
+      <c r="L15" s="55"/>
       <c r="M15" s="12"/>
     </row>
     <row r="16" spans="2:13" ht="86.4" x14ac:dyDescent="0.3">
@@ -2264,11 +2264,11 @@
       <c r="I19" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="J19" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
+      <c r="J19" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19" s="55"/>
+      <c r="L19" s="55"/>
       <c r="M19" s="12"/>
     </row>
     <row r="20" spans="2:13" ht="86.4" x14ac:dyDescent="0.3">
@@ -2572,10 +2572,10 @@
       <c r="D37" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="40" t="s">
+      <c r="E37" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="F37" s="40"/>
+      <c r="F37" s="56"/>
       <c r="G37" s="8" t="s">
         <v>20</v>
       </c>
@@ -2586,17 +2586,17 @@
       <c r="J37" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="K37" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="L37" s="43"/>
+      <c r="K37" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="L37" s="55"/>
       <c r="M37" s="12"/>
     </row>
     <row r="38" spans="2:13" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="E38" s="41" t="s">
+      <c r="E38" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="F38" s="41"/>
+      <c r="F38" s="44"/>
       <c r="G38" s="1">
         <v>0</v>
       </c>
@@ -2646,14 +2646,14 @@
       <c r="H42" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="I42" s="40" t="s">
+      <c r="I42" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="J42" s="40"/>
-      <c r="K42" s="40" t="s">
+      <c r="J42" s="56"/>
+      <c r="K42" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="L42" s="40"/>
+      <c r="L42" s="56"/>
       <c r="M42" s="12"/>
     </row>
     <row r="43" spans="2:13" ht="115.2" x14ac:dyDescent="0.3">
@@ -2669,14 +2669,14 @@
       <c r="H43" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="I43" s="41" t="s">
+      <c r="I43" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="J43" s="41"/>
-      <c r="K43" s="41" t="s">
+      <c r="J43" s="44"/>
+      <c r="K43" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="L43" s="41"/>
+      <c r="L43" s="44"/>
     </row>
     <row r="44" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E44" s="1" t="s">
@@ -2705,14 +2705,14 @@
       <c r="H46" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="I46" s="40" t="s">
+      <c r="I46" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="J46" s="40"/>
-      <c r="K46" s="40" t="s">
+      <c r="J46" s="56"/>
+      <c r="K46" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="L46" s="40"/>
+      <c r="L46" s="56"/>
       <c r="M46" s="12"/>
     </row>
     <row r="47" spans="2:13" ht="115.2" x14ac:dyDescent="0.3">
@@ -2728,14 +2728,14 @@
       <c r="H47" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="I47" s="41" t="s">
+      <c r="I47" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="J47" s="41"/>
-      <c r="K47" s="41" t="s">
+      <c r="J47" s="44"/>
+      <c r="K47" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="L47" s="41"/>
+      <c r="L47" s="44"/>
     </row>
     <row r="48" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E48" s="1" t="s">
@@ -2752,41 +2752,41 @@
       <c r="D50" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E50" s="40" t="s">
+      <c r="E50" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="F50" s="40"/>
-      <c r="G50" s="40" t="s">
+      <c r="F50" s="56"/>
+      <c r="G50" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="H50" s="40"/>
-      <c r="I50" s="40" t="s">
+      <c r="H50" s="56"/>
+      <c r="I50" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="J50" s="40"/>
-      <c r="K50" s="40" t="s">
+      <c r="J50" s="56"/>
+      <c r="K50" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="L50" s="40"/>
+      <c r="L50" s="56"/>
       <c r="M50" s="12"/>
     </row>
     <row r="51" spans="2:13" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E51" s="41" t="s">
+      <c r="E51" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="F51" s="41"/>
-      <c r="G51" s="41" t="s">
+      <c r="F51" s="44"/>
+      <c r="G51" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="H51" s="41"/>
-      <c r="I51" s="41" t="s">
+      <c r="H51" s="44"/>
+      <c r="I51" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="J51" s="41"/>
-      <c r="K51" s="41" t="s">
+      <c r="J51" s="44"/>
+      <c r="K51" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="L51" s="41"/>
+      <c r="L51" s="44"/>
     </row>
     <row r="53" spans="2:13" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D53" s="18"/>
@@ -2802,28 +2802,28 @@
       <c r="D54" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E54" s="46" t="s">
+      <c r="E54" s="52" t="s">
         <v>123</v>
       </c>
-      <c r="F54" s="46"/>
-      <c r="G54" s="46"/>
-      <c r="H54" s="46"/>
-      <c r="I54" s="46"/>
-      <c r="J54" s="46"/>
-      <c r="K54" s="46"/>
-      <c r="L54" s="46"/>
+      <c r="F54" s="52"/>
+      <c r="G54" s="52"/>
+      <c r="H54" s="52"/>
+      <c r="I54" s="52"/>
+      <c r="J54" s="52"/>
+      <c r="K54" s="52"/>
+      <c r="L54" s="52"/>
     </row>
     <row r="55" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E55" s="41" t="s">
+      <c r="E55" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="F55" s="41"/>
-      <c r="G55" s="41"/>
-      <c r="H55" s="41"/>
-      <c r="I55" s="41"/>
-      <c r="J55" s="41"/>
-      <c r="K55" s="41"/>
-      <c r="L55" s="41"/>
+      <c r="F55" s="44"/>
+      <c r="G55" s="44"/>
+      <c r="H55" s="44"/>
+      <c r="I55" s="44"/>
+      <c r="J55" s="44"/>
+      <c r="K55" s="44"/>
+      <c r="L55" s="44"/>
     </row>
     <row r="58" spans="2:13" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B58" s="2" t="s">
@@ -2835,20 +2835,20 @@
       <c r="D58" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E58" s="47" t="s">
+      <c r="E58" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="F58" s="43"/>
-      <c r="G58" s="43"/>
-      <c r="H58" s="43"/>
-      <c r="I58" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="J58" s="43"/>
-      <c r="K58" s="40" t="s">
+      <c r="F58" s="55"/>
+      <c r="G58" s="55"/>
+      <c r="H58" s="55"/>
+      <c r="I58" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="J58" s="55"/>
+      <c r="K58" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="L58" s="40"/>
+      <c r="L58" s="56"/>
       <c r="M58" s="12"/>
     </row>
     <row r="59" spans="2:13" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2858,10 +2858,10 @@
       <c r="J59" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="K59" s="41" t="s">
+      <c r="K59" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="L59" s="41"/>
+      <c r="L59" s="44"/>
     </row>
     <row r="61" spans="2:13" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B61" s="2" t="s">
@@ -2873,29 +2873,29 @@
       <c r="D61" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E61" s="45" t="s">
+      <c r="E61" s="58" t="s">
         <v>130</v>
       </c>
-      <c r="F61" s="40"/>
-      <c r="G61" s="40"/>
-      <c r="H61" s="40"/>
-      <c r="I61" s="40"/>
-      <c r="J61" s="40"/>
-      <c r="K61" s="40"/>
-      <c r="L61" s="40"/>
+      <c r="F61" s="56"/>
+      <c r="G61" s="56"/>
+      <c r="H61" s="56"/>
+      <c r="I61" s="56"/>
+      <c r="J61" s="56"/>
+      <c r="K61" s="56"/>
+      <c r="L61" s="56"/>
       <c r="M61" s="12"/>
     </row>
     <row r="62" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E62" s="44" t="s">
+      <c r="E62" s="43" t="s">
         <v>138</v>
       </c>
-      <c r="F62" s="41"/>
-      <c r="G62" s="41"/>
-      <c r="H62" s="41"/>
-      <c r="I62" s="41"/>
-      <c r="J62" s="41"/>
-      <c r="K62" s="41"/>
-      <c r="L62" s="41"/>
+      <c r="F62" s="44"/>
+      <c r="G62" s="44"/>
+      <c r="H62" s="44"/>
+      <c r="I62" s="44"/>
+      <c r="J62" s="44"/>
+      <c r="K62" s="44"/>
+      <c r="L62" s="44"/>
     </row>
     <row r="65" spans="2:13" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B65" s="2" t="s">
@@ -2907,34 +2907,34 @@
       <c r="D65" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E65" s="45" t="s">
+      <c r="E65" s="58" t="s">
         <v>132</v>
       </c>
-      <c r="F65" s="40"/>
-      <c r="G65" s="40"/>
-      <c r="H65" s="40"/>
-      <c r="I65" s="40" t="s">
+      <c r="F65" s="56"/>
+      <c r="G65" s="56"/>
+      <c r="H65" s="56"/>
+      <c r="I65" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="J65" s="40"/>
-      <c r="K65" s="40"/>
-      <c r="L65" s="40"/>
+      <c r="J65" s="56"/>
+      <c r="K65" s="56"/>
+      <c r="L65" s="56"/>
       <c r="M65" s="12"/>
     </row>
     <row r="66" spans="2:13" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D66" s="1"/>
-      <c r="E66" s="44" t="s">
+      <c r="E66" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="F66" s="41"/>
-      <c r="G66" s="41"/>
-      <c r="H66" s="41"/>
-      <c r="I66" s="41" t="s">
+      <c r="F66" s="44"/>
+      <c r="G66" s="44"/>
+      <c r="H66" s="44"/>
+      <c r="I66" s="44" t="s">
         <v>140</v>
       </c>
-      <c r="J66" s="41"/>
-      <c r="K66" s="41"/>
-      <c r="L66" s="41"/>
+      <c r="J66" s="44"/>
+      <c r="K66" s="44"/>
+      <c r="L66" s="44"/>
     </row>
     <row r="69" spans="2:13" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B69" s="2" t="s">
@@ -2946,29 +2946,29 @@
       <c r="D69" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E69" s="45" t="s">
+      <c r="E69" s="58" t="s">
         <v>137</v>
       </c>
-      <c r="F69" s="40"/>
-      <c r="G69" s="40"/>
-      <c r="H69" s="40"/>
-      <c r="I69" s="40"/>
-      <c r="J69" s="40"/>
-      <c r="K69" s="40"/>
-      <c r="L69" s="40"/>
+      <c r="F69" s="56"/>
+      <c r="G69" s="56"/>
+      <c r="H69" s="56"/>
+      <c r="I69" s="56"/>
+      <c r="J69" s="56"/>
+      <c r="K69" s="56"/>
+      <c r="L69" s="56"/>
       <c r="M69" s="12"/>
     </row>
     <row r="70" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E70" s="44" t="s">
+      <c r="E70" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="F70" s="41"/>
-      <c r="G70" s="41"/>
-      <c r="H70" s="41"/>
-      <c r="I70" s="41"/>
-      <c r="J70" s="41"/>
-      <c r="K70" s="41"/>
-      <c r="L70" s="41"/>
+      <c r="F70" s="44"/>
+      <c r="G70" s="44"/>
+      <c r="H70" s="44"/>
+      <c r="I70" s="44"/>
+      <c r="J70" s="44"/>
+      <c r="K70" s="44"/>
+      <c r="L70" s="44"/>
     </row>
     <row r="72" spans="2:13" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D72" s="18"/>
@@ -2984,28 +2984,28 @@
       <c r="D73" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E73" s="46" t="s">
+      <c r="E73" s="52" t="s">
         <v>144</v>
       </c>
-      <c r="F73" s="46"/>
-      <c r="G73" s="46"/>
-      <c r="H73" s="46"/>
-      <c r="I73" s="46"/>
-      <c r="J73" s="46"/>
-      <c r="K73" s="46"/>
-      <c r="L73" s="46"/>
+      <c r="F73" s="52"/>
+      <c r="G73" s="52"/>
+      <c r="H73" s="52"/>
+      <c r="I73" s="52"/>
+      <c r="J73" s="52"/>
+      <c r="K73" s="52"/>
+      <c r="L73" s="52"/>
     </row>
     <row r="74" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E74" s="41" t="s">
+      <c r="E74" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="F74" s="41"/>
-      <c r="G74" s="41"/>
-      <c r="H74" s="41"/>
-      <c r="I74" s="41"/>
-      <c r="J74" s="41"/>
-      <c r="K74" s="41"/>
-      <c r="L74" s="41"/>
+      <c r="F74" s="44"/>
+      <c r="G74" s="44"/>
+      <c r="H74" s="44"/>
+      <c r="I74" s="44"/>
+      <c r="J74" s="44"/>
+      <c r="K74" s="44"/>
+      <c r="L74" s="44"/>
     </row>
     <row r="77" spans="2:13" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B77" s="2" t="s">
@@ -3017,20 +3017,20 @@
       <c r="D77" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E77" s="47" t="s">
+      <c r="E77" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="F77" s="43"/>
-      <c r="G77" s="43"/>
-      <c r="H77" s="43"/>
-      <c r="I77" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="J77" s="43"/>
-      <c r="K77" s="40" t="s">
+      <c r="F77" s="55"/>
+      <c r="G77" s="55"/>
+      <c r="H77" s="55"/>
+      <c r="I77" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="J77" s="55"/>
+      <c r="K77" s="56" t="s">
         <v>149</v>
       </c>
-      <c r="L77" s="40"/>
+      <c r="L77" s="56"/>
       <c r="M77" s="12"/>
     </row>
     <row r="78" spans="2:13" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3040,10 +3040,10 @@
       <c r="J78" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="K78" s="41" t="s">
+      <c r="K78" s="44" t="s">
         <v>148</v>
       </c>
-      <c r="L78" s="41"/>
+      <c r="L78" s="44"/>
     </row>
     <row r="80" spans="2:13" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B80" s="2" t="s">
@@ -3055,29 +3055,29 @@
       <c r="D80" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E80" s="45" t="s">
+      <c r="E80" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="F80" s="40"/>
-      <c r="G80" s="40"/>
-      <c r="H80" s="40"/>
-      <c r="I80" s="40"/>
-      <c r="J80" s="40"/>
-      <c r="K80" s="40"/>
-      <c r="L80" s="40"/>
+      <c r="F80" s="56"/>
+      <c r="G80" s="56"/>
+      <c r="H80" s="56"/>
+      <c r="I80" s="56"/>
+      <c r="J80" s="56"/>
+      <c r="K80" s="56"/>
+      <c r="L80" s="56"/>
       <c r="M80" s="12"/>
     </row>
     <row r="81" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E81" s="44" t="s">
+      <c r="E81" s="43" t="s">
         <v>148</v>
       </c>
-      <c r="F81" s="41"/>
-      <c r="G81" s="41"/>
-      <c r="H81" s="41"/>
-      <c r="I81" s="41"/>
-      <c r="J81" s="41"/>
-      <c r="K81" s="41"/>
-      <c r="L81" s="41"/>
+      <c r="F81" s="44"/>
+      <c r="G81" s="44"/>
+      <c r="H81" s="44"/>
+      <c r="I81" s="44"/>
+      <c r="J81" s="44"/>
+      <c r="K81" s="44"/>
+      <c r="L81" s="44"/>
     </row>
     <row r="84" spans="2:13" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B84" s="2" t="s">
@@ -3089,34 +3089,34 @@
       <c r="D84" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E84" s="45" t="s">
+      <c r="E84" s="58" t="s">
         <v>155</v>
       </c>
-      <c r="F84" s="40"/>
-      <c r="G84" s="40"/>
-      <c r="H84" s="40"/>
-      <c r="I84" s="40" t="s">
+      <c r="F84" s="56"/>
+      <c r="G84" s="56"/>
+      <c r="H84" s="56"/>
+      <c r="I84" s="56" t="s">
         <v>156</v>
       </c>
-      <c r="J84" s="40"/>
-      <c r="K84" s="40"/>
-      <c r="L84" s="40"/>
+      <c r="J84" s="56"/>
+      <c r="K84" s="56"/>
+      <c r="L84" s="56"/>
       <c r="M84" s="12"/>
     </row>
     <row r="85" spans="2:13" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D85" s="1"/>
-      <c r="E85" s="44" t="s">
+      <c r="E85" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="F85" s="41"/>
-      <c r="G85" s="41"/>
-      <c r="H85" s="41"/>
-      <c r="I85" s="41" t="s">
+      <c r="F85" s="44"/>
+      <c r="G85" s="44"/>
+      <c r="H85" s="44"/>
+      <c r="I85" s="44" t="s">
         <v>157</v>
       </c>
-      <c r="J85" s="41"/>
-      <c r="K85" s="41"/>
-      <c r="L85" s="41"/>
+      <c r="J85" s="44"/>
+      <c r="K85" s="44"/>
+      <c r="L85" s="44"/>
     </row>
     <row r="88" spans="2:13" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B88" s="2" t="s">
@@ -3128,29 +3128,29 @@
       <c r="D88" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E88" s="45" t="s">
+      <c r="E88" s="58" t="s">
         <v>160</v>
       </c>
-      <c r="F88" s="40"/>
-      <c r="G88" s="40"/>
-      <c r="H88" s="40"/>
-      <c r="I88" s="40"/>
-      <c r="J88" s="40"/>
-      <c r="K88" s="40"/>
-      <c r="L88" s="40"/>
+      <c r="F88" s="56"/>
+      <c r="G88" s="56"/>
+      <c r="H88" s="56"/>
+      <c r="I88" s="56"/>
+      <c r="J88" s="56"/>
+      <c r="K88" s="56"/>
+      <c r="L88" s="56"/>
       <c r="M88" s="12"/>
     </row>
     <row r="89" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E89" s="44" t="s">
+      <c r="E89" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="F89" s="41"/>
-      <c r="G89" s="41"/>
-      <c r="H89" s="41"/>
-      <c r="I89" s="41"/>
-      <c r="J89" s="41"/>
-      <c r="K89" s="41"/>
-      <c r="L89" s="41"/>
+      <c r="F89" s="44"/>
+      <c r="G89" s="44"/>
+      <c r="H89" s="44"/>
+      <c r="I89" s="44"/>
+      <c r="J89" s="44"/>
+      <c r="K89" s="44"/>
+      <c r="L89" s="44"/>
     </row>
     <row r="91" spans="2:13" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D91" s="18"/>
@@ -3166,16 +3166,16 @@
       <c r="D92" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E92" s="48" t="s">
+      <c r="E92" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="F92" s="49"/>
-      <c r="G92" s="49"/>
-      <c r="H92" s="49"/>
-      <c r="I92" s="49"/>
-      <c r="J92" s="49"/>
-      <c r="K92" s="49"/>
-      <c r="L92" s="49"/>
+      <c r="F92" s="46"/>
+      <c r="G92" s="46"/>
+      <c r="H92" s="46"/>
+      <c r="I92" s="46"/>
+      <c r="J92" s="46"/>
+      <c r="K92" s="46"/>
+      <c r="L92" s="46"/>
     </row>
     <row r="95" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D95" s="20"/>
@@ -3194,34 +3194,34 @@
       <c r="E96" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="F96" s="40" t="s">
+      <c r="F96" s="56" t="s">
         <v>166</v>
       </c>
-      <c r="G96" s="40"/>
-      <c r="H96" s="40"/>
-      <c r="I96" s="40" t="s">
+      <c r="G96" s="56"/>
+      <c r="H96" s="56"/>
+      <c r="I96" s="56" t="s">
         <v>168</v>
       </c>
-      <c r="J96" s="40"/>
-      <c r="K96" s="40" t="s">
+      <c r="J96" s="56"/>
+      <c r="K96" s="56" t="s">
         <v>169</v>
       </c>
-      <c r="L96" s="40"/>
+      <c r="L96" s="56"/>
     </row>
     <row r="97" spans="2:13" ht="115.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F97" s="41" t="s">
+      <c r="F97" s="44" t="s">
         <v>172</v>
       </c>
-      <c r="G97" s="41"/>
-      <c r="H97" s="41"/>
-      <c r="I97" s="41" t="s">
+      <c r="G97" s="44"/>
+      <c r="H97" s="44"/>
+      <c r="I97" s="44" t="s">
         <v>170</v>
       </c>
-      <c r="J97" s="41"/>
-      <c r="K97" s="41" t="s">
+      <c r="J97" s="44"/>
+      <c r="K97" s="44" t="s">
         <v>171</v>
       </c>
-      <c r="L97" s="41"/>
+      <c r="L97" s="44"/>
     </row>
     <row r="99" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D99" s="20"/>
@@ -3237,28 +3237,28 @@
       <c r="D100" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E100" s="45" t="s">
+      <c r="E100" s="58" t="s">
         <v>175</v>
       </c>
-      <c r="F100" s="40"/>
-      <c r="G100" s="40"/>
-      <c r="H100" s="40"/>
-      <c r="I100" s="40"/>
-      <c r="J100" s="40"/>
-      <c r="K100" s="40"/>
-      <c r="L100" s="40"/>
+      <c r="F100" s="56"/>
+      <c r="G100" s="56"/>
+      <c r="H100" s="56"/>
+      <c r="I100" s="56"/>
+      <c r="J100" s="56"/>
+      <c r="K100" s="56"/>
+      <c r="L100" s="56"/>
     </row>
     <row r="101" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E101" s="44" t="s">
+      <c r="E101" s="43" t="s">
         <v>171</v>
       </c>
-      <c r="F101" s="41"/>
-      <c r="G101" s="41"/>
-      <c r="H101" s="41"/>
-      <c r="I101" s="41"/>
-      <c r="J101" s="41"/>
-      <c r="K101" s="41"/>
-      <c r="L101" s="41"/>
+      <c r="F101" s="44"/>
+      <c r="G101" s="44"/>
+      <c r="H101" s="44"/>
+      <c r="I101" s="44"/>
+      <c r="J101" s="44"/>
+      <c r="K101" s="44"/>
+      <c r="L101" s="44"/>
     </row>
     <row r="103" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D103" s="20"/>
@@ -3274,32 +3274,32 @@
       <c r="D104" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E104" s="45" t="s">
+      <c r="E104" s="58" t="s">
         <v>178</v>
       </c>
-      <c r="F104" s="40"/>
-      <c r="G104" s="40"/>
-      <c r="H104" s="40"/>
-      <c r="I104" s="40" t="s">
+      <c r="F104" s="56"/>
+      <c r="G104" s="56"/>
+      <c r="H104" s="56"/>
+      <c r="I104" s="56" t="s">
         <v>179</v>
       </c>
-      <c r="J104" s="40"/>
-      <c r="K104" s="40"/>
-      <c r="L104" s="40"/>
+      <c r="J104" s="56"/>
+      <c r="K104" s="56"/>
+      <c r="L104" s="56"/>
     </row>
     <row r="105" spans="2:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E105" s="44" t="s">
+      <c r="E105" s="43" t="s">
         <v>180</v>
       </c>
-      <c r="F105" s="41"/>
-      <c r="G105" s="41"/>
-      <c r="H105" s="41"/>
-      <c r="I105" s="41" t="s">
+      <c r="F105" s="44"/>
+      <c r="G105" s="44"/>
+      <c r="H105" s="44"/>
+      <c r="I105" s="44" t="s">
         <v>181</v>
       </c>
-      <c r="J105" s="41"/>
-      <c r="K105" s="41"/>
-      <c r="L105" s="41"/>
+      <c r="J105" s="44"/>
+      <c r="K105" s="44"/>
+      <c r="L105" s="44"/>
     </row>
     <row r="107" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D107" s="20"/>
@@ -3315,28 +3315,28 @@
       <c r="D108" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E108" s="45" t="s">
+      <c r="E108" s="58" t="s">
         <v>184</v>
       </c>
-      <c r="F108" s="40"/>
-      <c r="G108" s="40"/>
-      <c r="H108" s="40"/>
-      <c r="I108" s="40"/>
-      <c r="J108" s="40"/>
-      <c r="K108" s="40"/>
-      <c r="L108" s="40"/>
+      <c r="F108" s="56"/>
+      <c r="G108" s="56"/>
+      <c r="H108" s="56"/>
+      <c r="I108" s="56"/>
+      <c r="J108" s="56"/>
+      <c r="K108" s="56"/>
+      <c r="L108" s="56"/>
     </row>
     <row r="109" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E109" s="44" t="s">
+      <c r="E109" s="43" t="s">
         <v>181</v>
       </c>
-      <c r="F109" s="41"/>
-      <c r="G109" s="41"/>
-      <c r="H109" s="41"/>
-      <c r="I109" s="41"/>
-      <c r="J109" s="41"/>
-      <c r="K109" s="41"/>
-      <c r="L109" s="41"/>
+      <c r="F109" s="44"/>
+      <c r="G109" s="44"/>
+      <c r="H109" s="44"/>
+      <c r="I109" s="44"/>
+      <c r="J109" s="44"/>
+      <c r="K109" s="44"/>
+      <c r="L109" s="44"/>
     </row>
     <row r="111" spans="2:13" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D111" s="18"/>
@@ -3349,16 +3349,16 @@
       <c r="C112" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E112" s="48" t="s">
+      <c r="E112" s="50" t="s">
         <v>187</v>
       </c>
-      <c r="F112" s="49"/>
-      <c r="G112" s="49"/>
-      <c r="H112" s="49"/>
-      <c r="I112" s="49"/>
-      <c r="J112" s="49"/>
-      <c r="K112" s="49"/>
-      <c r="L112" s="49"/>
+      <c r="F112" s="46"/>
+      <c r="G112" s="46"/>
+      <c r="H112" s="46"/>
+      <c r="I112" s="46"/>
+      <c r="J112" s="46"/>
+      <c r="K112" s="46"/>
+      <c r="L112" s="46"/>
     </row>
     <row r="115" spans="2:13" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D115" s="18"/>
@@ -3374,28 +3374,28 @@
       <c r="D116" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E116" s="48" t="s">
+      <c r="E116" s="50" t="s">
         <v>191</v>
       </c>
-      <c r="F116" s="49"/>
-      <c r="G116" s="49"/>
-      <c r="H116" s="49"/>
-      <c r="I116" s="49"/>
-      <c r="J116" s="49"/>
-      <c r="K116" s="49"/>
-      <c r="L116" s="49"/>
+      <c r="F116" s="46"/>
+      <c r="G116" s="46"/>
+      <c r="H116" s="46"/>
+      <c r="I116" s="46"/>
+      <c r="J116" s="46"/>
+      <c r="K116" s="46"/>
+      <c r="L116" s="46"/>
     </row>
     <row r="117" spans="2:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E117" s="44" t="s">
+      <c r="E117" s="43" t="s">
         <v>188</v>
       </c>
-      <c r="F117" s="41"/>
-      <c r="G117" s="41"/>
-      <c r="H117" s="41"/>
-      <c r="I117" s="41"/>
-      <c r="J117" s="41"/>
-      <c r="K117" s="41"/>
-      <c r="L117" s="41"/>
+      <c r="F117" s="44"/>
+      <c r="G117" s="44"/>
+      <c r="H117" s="44"/>
+      <c r="I117" s="44"/>
+      <c r="J117" s="44"/>
+      <c r="K117" s="44"/>
+      <c r="L117" s="44"/>
     </row>
     <row r="119" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D119" s="20"/>
@@ -3414,31 +3414,31 @@
       <c r="E120" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F120" s="40" t="s">
+      <c r="F120" s="56" t="s">
         <v>193</v>
       </c>
-      <c r="G120" s="40"/>
-      <c r="H120" s="40"/>
+      <c r="G120" s="56"/>
+      <c r="H120" s="56"/>
       <c r="I120" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J120" s="40" t="s">
+      <c r="J120" s="56" t="s">
         <v>195</v>
       </c>
-      <c r="K120" s="40"/>
-      <c r="L120" s="40"/>
+      <c r="K120" s="56"/>
+      <c r="L120" s="56"/>
     </row>
     <row r="121" spans="2:13" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F121" s="41" t="s">
+      <c r="F121" s="44" t="s">
         <v>172</v>
       </c>
-      <c r="G121" s="41"/>
-      <c r="H121" s="41"/>
-      <c r="J121" s="41" t="s">
+      <c r="G121" s="44"/>
+      <c r="H121" s="44"/>
+      <c r="J121" s="44" t="s">
         <v>172</v>
       </c>
-      <c r="K121" s="41"/>
-      <c r="L121" s="41"/>
+      <c r="K121" s="44"/>
+      <c r="L121" s="44"/>
     </row>
     <row r="123" spans="2:13" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D123" s="18"/>
@@ -3454,16 +3454,16 @@
       <c r="D124" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E124" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F124" s="53"/>
-      <c r="G124" s="53"/>
-      <c r="H124" s="53"/>
-      <c r="I124" s="53"/>
-      <c r="J124" s="53"/>
-      <c r="K124" s="53"/>
-      <c r="L124" s="53"/>
+      <c r="E124" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F124" s="41"/>
+      <c r="G124" s="41"/>
+      <c r="H124" s="41"/>
+      <c r="I124" s="41"/>
+      <c r="J124" s="41"/>
+      <c r="K124" s="41"/>
+      <c r="L124" s="41"/>
     </row>
     <row r="127" spans="2:13" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D127" s="18"/>
@@ -3482,29 +3482,29 @@
       <c r="E128" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="F128" s="49" t="s">
+      <c r="F128" s="46" t="s">
         <v>202</v>
       </c>
-      <c r="G128" s="49"/>
-      <c r="H128" s="49"/>
-      <c r="I128" s="49"/>
-      <c r="J128" s="49"/>
-      <c r="K128" s="49"/>
-      <c r="L128" s="49"/>
+      <c r="G128" s="46"/>
+      <c r="H128" s="46"/>
+      <c r="I128" s="46"/>
+      <c r="J128" s="46"/>
+      <c r="K128" s="46"/>
+      <c r="L128" s="46"/>
     </row>
     <row r="129" spans="2:13" x14ac:dyDescent="0.3">
       <c r="E129" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="F129" s="41" t="s">
+      <c r="F129" s="44" t="s">
         <v>203</v>
       </c>
-      <c r="G129" s="41"/>
-      <c r="H129" s="41"/>
-      <c r="I129" s="41"/>
-      <c r="J129" s="41"/>
-      <c r="K129" s="41"/>
-      <c r="L129" s="41"/>
+      <c r="G129" s="44"/>
+      <c r="H129" s="44"/>
+      <c r="I129" s="44"/>
+      <c r="J129" s="44"/>
+      <c r="K129" s="44"/>
+      <c r="L129" s="44"/>
     </row>
     <row r="130" spans="2:13" ht="72" x14ac:dyDescent="0.3">
       <c r="E130" s="1" t="s">
@@ -3525,28 +3525,28 @@
       <c r="D132" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E132" s="45" t="s">
+      <c r="E132" s="58" t="s">
         <v>206</v>
       </c>
-      <c r="F132" s="40"/>
-      <c r="G132" s="40"/>
-      <c r="H132" s="40"/>
-      <c r="I132" s="40"/>
-      <c r="J132" s="40"/>
-      <c r="K132" s="40"/>
-      <c r="L132" s="40"/>
+      <c r="F132" s="56"/>
+      <c r="G132" s="56"/>
+      <c r="H132" s="56"/>
+      <c r="I132" s="56"/>
+      <c r="J132" s="56"/>
+      <c r="K132" s="56"/>
+      <c r="L132" s="56"/>
     </row>
     <row r="133" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E133" s="44" t="s">
+      <c r="E133" s="43" t="s">
         <v>207</v>
       </c>
-      <c r="F133" s="41"/>
-      <c r="G133" s="41"/>
-      <c r="H133" s="41"/>
-      <c r="I133" s="41"/>
-      <c r="J133" s="41"/>
-      <c r="K133" s="41"/>
-      <c r="L133" s="50"/>
+      <c r="F133" s="44"/>
+      <c r="G133" s="44"/>
+      <c r="H133" s="44"/>
+      <c r="I133" s="44"/>
+      <c r="J133" s="44"/>
+      <c r="K133" s="44"/>
+      <c r="L133" s="45"/>
     </row>
     <row r="135" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D135" s="20"/>
@@ -3566,29 +3566,29 @@
       <c r="E136" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="F136" s="40" t="s">
+      <c r="F136" s="56" t="s">
         <v>212</v>
       </c>
-      <c r="G136" s="40"/>
-      <c r="H136" s="40"/>
-      <c r="I136" s="40"/>
-      <c r="J136" s="40"/>
-      <c r="K136" s="40"/>
-      <c r="L136" s="51"/>
+      <c r="G136" s="56"/>
+      <c r="H136" s="56"/>
+      <c r="I136" s="56"/>
+      <c r="J136" s="56"/>
+      <c r="K136" s="56"/>
+      <c r="L136" s="57"/>
     </row>
     <row r="137" spans="2:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="E137" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="F137" s="41" t="s">
+      <c r="F137" s="44" t="s">
         <v>213</v>
       </c>
-      <c r="G137" s="41"/>
-      <c r="H137" s="41"/>
-      <c r="I137" s="41"/>
-      <c r="J137" s="41"/>
-      <c r="K137" s="41"/>
-      <c r="L137" s="50"/>
+      <c r="G137" s="44"/>
+      <c r="H137" s="44"/>
+      <c r="I137" s="44"/>
+      <c r="J137" s="44"/>
+      <c r="K137" s="44"/>
+      <c r="L137" s="45"/>
     </row>
     <row r="139" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D139" s="20"/>
@@ -3604,28 +3604,28 @@
       <c r="D140" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E140" s="45" t="s">
+      <c r="E140" s="58" t="s">
         <v>216</v>
       </c>
-      <c r="F140" s="40"/>
-      <c r="G140" s="40"/>
-      <c r="H140" s="40"/>
-      <c r="I140" s="40"/>
-      <c r="J140" s="40"/>
-      <c r="K140" s="40"/>
-      <c r="L140" s="51"/>
+      <c r="F140" s="56"/>
+      <c r="G140" s="56"/>
+      <c r="H140" s="56"/>
+      <c r="I140" s="56"/>
+      <c r="J140" s="56"/>
+      <c r="K140" s="56"/>
+      <c r="L140" s="57"/>
     </row>
     <row r="141" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E141" s="44" t="s">
+      <c r="E141" s="43" t="s">
         <v>217</v>
       </c>
-      <c r="F141" s="41"/>
-      <c r="G141" s="41"/>
-      <c r="H141" s="41"/>
-      <c r="I141" s="41"/>
-      <c r="J141" s="41"/>
-      <c r="K141" s="41"/>
-      <c r="L141" s="50"/>
+      <c r="F141" s="44"/>
+      <c r="G141" s="44"/>
+      <c r="H141" s="44"/>
+      <c r="I141" s="44"/>
+      <c r="J141" s="44"/>
+      <c r="K141" s="44"/>
+      <c r="L141" s="45"/>
     </row>
     <row r="143" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D143" s="20"/>
@@ -3641,28 +3641,28 @@
       <c r="D144" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E144" s="45" t="s">
+      <c r="E144" s="58" t="s">
         <v>219</v>
       </c>
-      <c r="F144" s="40"/>
-      <c r="G144" s="40"/>
-      <c r="H144" s="40"/>
-      <c r="I144" s="40"/>
-      <c r="J144" s="40"/>
-      <c r="K144" s="40"/>
-      <c r="L144" s="51"/>
+      <c r="F144" s="56"/>
+      <c r="G144" s="56"/>
+      <c r="H144" s="56"/>
+      <c r="I144" s="56"/>
+      <c r="J144" s="56"/>
+      <c r="K144" s="56"/>
+      <c r="L144" s="57"/>
     </row>
     <row r="145" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E145" s="44" t="s">
+      <c r="E145" s="43" t="s">
         <v>220</v>
       </c>
-      <c r="F145" s="41"/>
-      <c r="G145" s="41"/>
-      <c r="H145" s="41"/>
-      <c r="I145" s="41"/>
-      <c r="J145" s="41"/>
-      <c r="K145" s="41"/>
-      <c r="L145" s="50"/>
+      <c r="F145" s="44"/>
+      <c r="G145" s="44"/>
+      <c r="H145" s="44"/>
+      <c r="I145" s="44"/>
+      <c r="J145" s="44"/>
+      <c r="K145" s="44"/>
+      <c r="L145" s="45"/>
     </row>
     <row r="147" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D147" s="20"/>
@@ -3678,28 +3678,28 @@
       <c r="D148" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E148" s="45" t="s">
+      <c r="E148" s="58" t="s">
         <v>223</v>
       </c>
-      <c r="F148" s="40"/>
-      <c r="G148" s="40"/>
-      <c r="H148" s="40"/>
-      <c r="I148" s="40" t="s">
+      <c r="F148" s="56"/>
+      <c r="G148" s="56"/>
+      <c r="H148" s="56"/>
+      <c r="I148" s="56" t="s">
         <v>224</v>
       </c>
-      <c r="J148" s="40"/>
-      <c r="K148" s="40"/>
-      <c r="L148" s="51"/>
+      <c r="J148" s="56"/>
+      <c r="K148" s="56"/>
+      <c r="L148" s="57"/>
     </row>
     <row r="149" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E149" s="44"/>
-      <c r="F149" s="41"/>
-      <c r="G149" s="41"/>
-      <c r="H149" s="41"/>
-      <c r="I149" s="41"/>
-      <c r="J149" s="41"/>
-      <c r="K149" s="41"/>
-      <c r="L149" s="50"/>
+      <c r="E149" s="43"/>
+      <c r="F149" s="44"/>
+      <c r="G149" s="44"/>
+      <c r="H149" s="44"/>
+      <c r="I149" s="44"/>
+      <c r="J149" s="44"/>
+      <c r="K149" s="44"/>
+      <c r="L149" s="45"/>
     </row>
     <row r="151" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D151" s="20"/>
@@ -3715,26 +3715,26 @@
       <c r="D152" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E152" s="45" t="s">
+      <c r="E152" s="58" t="s">
         <v>227</v>
       </c>
-      <c r="F152" s="40"/>
-      <c r="G152" s="40"/>
-      <c r="H152" s="40"/>
-      <c r="I152" s="40"/>
-      <c r="J152" s="40"/>
-      <c r="K152" s="40"/>
-      <c r="L152" s="51"/>
+      <c r="F152" s="56"/>
+      <c r="G152" s="56"/>
+      <c r="H152" s="56"/>
+      <c r="I152" s="56"/>
+      <c r="J152" s="56"/>
+      <c r="K152" s="56"/>
+      <c r="L152" s="57"/>
     </row>
     <row r="153" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E153" s="44"/>
-      <c r="F153" s="41"/>
-      <c r="G153" s="41"/>
-      <c r="H153" s="41"/>
-      <c r="I153" s="41"/>
-      <c r="J153" s="41"/>
-      <c r="K153" s="41"/>
-      <c r="L153" s="50"/>
+      <c r="E153" s="43"/>
+      <c r="F153" s="44"/>
+      <c r="G153" s="44"/>
+      <c r="H153" s="44"/>
+      <c r="I153" s="44"/>
+      <c r="J153" s="44"/>
+      <c r="K153" s="44"/>
+      <c r="L153" s="45"/>
     </row>
     <row r="155" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D155" s="20"/>
@@ -3753,26 +3753,26 @@
       <c r="E156" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="F156" s="40" t="s">
+      <c r="F156" s="56" t="s">
         <v>233</v>
       </c>
-      <c r="G156" s="40"/>
-      <c r="H156" s="40"/>
-      <c r="I156" s="40"/>
-      <c r="J156" s="40"/>
-      <c r="K156" s="40"/>
-      <c r="L156" s="51"/>
+      <c r="G156" s="56"/>
+      <c r="H156" s="56"/>
+      <c r="I156" s="56"/>
+      <c r="J156" s="56"/>
+      <c r="K156" s="56"/>
+      <c r="L156" s="57"/>
     </row>
     <row r="157" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F157" s="41" t="s">
+      <c r="F157" s="44" t="s">
         <v>234</v>
       </c>
-      <c r="G157" s="41"/>
-      <c r="H157" s="41"/>
-      <c r="I157" s="41"/>
-      <c r="J157" s="41"/>
-      <c r="K157" s="41"/>
-      <c r="L157" s="50"/>
+      <c r="G157" s="44"/>
+      <c r="H157" s="44"/>
+      <c r="I157" s="44"/>
+      <c r="J157" s="44"/>
+      <c r="K157" s="44"/>
+      <c r="L157" s="45"/>
     </row>
     <row r="159" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D159" s="20"/>
@@ -3788,28 +3788,28 @@
       <c r="D160" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E160" s="45" t="s">
+      <c r="E160" s="58" t="s">
         <v>230</v>
       </c>
-      <c r="F160" s="40"/>
-      <c r="G160" s="40"/>
-      <c r="H160" s="40"/>
-      <c r="I160" s="40"/>
-      <c r="J160" s="40"/>
-      <c r="K160" s="40"/>
-      <c r="L160" s="51"/>
+      <c r="F160" s="56"/>
+      <c r="G160" s="56"/>
+      <c r="H160" s="56"/>
+      <c r="I160" s="56"/>
+      <c r="J160" s="56"/>
+      <c r="K160" s="56"/>
+      <c r="L160" s="57"/>
     </row>
     <row r="161" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E161" s="44" t="s">
+      <c r="E161" s="43" t="s">
         <v>231</v>
       </c>
-      <c r="F161" s="41"/>
-      <c r="G161" s="41"/>
-      <c r="H161" s="41"/>
-      <c r="I161" s="41"/>
-      <c r="J161" s="41"/>
-      <c r="K161" s="41"/>
-      <c r="L161" s="50"/>
+      <c r="F161" s="44"/>
+      <c r="G161" s="44"/>
+      <c r="H161" s="44"/>
+      <c r="I161" s="44"/>
+      <c r="J161" s="44"/>
+      <c r="K161" s="44"/>
+      <c r="L161" s="45"/>
     </row>
     <row r="163" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D163" s="20"/>
@@ -3828,26 +3828,26 @@
       <c r="E164" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="F164" s="40" t="s">
+      <c r="F164" s="56" t="s">
         <v>238</v>
       </c>
-      <c r="G164" s="40"/>
-      <c r="H164" s="40"/>
-      <c r="I164" s="40"/>
-      <c r="J164" s="40"/>
-      <c r="K164" s="40"/>
-      <c r="L164" s="51"/>
+      <c r="G164" s="56"/>
+      <c r="H164" s="56"/>
+      <c r="I164" s="56"/>
+      <c r="J164" s="56"/>
+      <c r="K164" s="56"/>
+      <c r="L164" s="57"/>
     </row>
     <row r="165" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F165" s="41" t="s">
+      <c r="F165" s="44" t="s">
         <v>239</v>
       </c>
-      <c r="G165" s="41"/>
-      <c r="H165" s="41"/>
-      <c r="I165" s="41"/>
-      <c r="J165" s="41"/>
-      <c r="K165" s="41"/>
-      <c r="L165" s="50"/>
+      <c r="G165" s="44"/>
+      <c r="H165" s="44"/>
+      <c r="I165" s="44"/>
+      <c r="J165" s="44"/>
+      <c r="K165" s="44"/>
+      <c r="L165" s="45"/>
     </row>
     <row r="167" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D167" s="20"/>
@@ -3863,28 +3863,28 @@
       <c r="D168" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E168" s="55" t="s">
+      <c r="E168" s="51" t="s">
         <v>241</v>
       </c>
-      <c r="F168" s="46"/>
-      <c r="G168" s="46"/>
-      <c r="H168" s="46"/>
-      <c r="I168" s="46"/>
-      <c r="J168" s="46"/>
-      <c r="K168" s="46"/>
-      <c r="L168" s="56"/>
+      <c r="F168" s="52"/>
+      <c r="G168" s="52"/>
+      <c r="H168" s="52"/>
+      <c r="I168" s="52"/>
+      <c r="J168" s="52"/>
+      <c r="K168" s="52"/>
+      <c r="L168" s="53"/>
     </row>
     <row r="169" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E169" s="44" t="s">
+      <c r="E169" s="43" t="s">
         <v>242</v>
       </c>
-      <c r="F169" s="41"/>
-      <c r="G169" s="41"/>
-      <c r="H169" s="41"/>
-      <c r="I169" s="41"/>
-      <c r="J169" s="41"/>
-      <c r="K169" s="41"/>
-      <c r="L169" s="50"/>
+      <c r="F169" s="44"/>
+      <c r="G169" s="44"/>
+      <c r="H169" s="44"/>
+      <c r="I169" s="44"/>
+      <c r="J169" s="44"/>
+      <c r="K169" s="44"/>
+      <c r="L169" s="45"/>
     </row>
     <row r="171" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D171" s="20"/>
@@ -3900,28 +3900,28 @@
       <c r="D172" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E172" s="45" t="s">
+      <c r="E172" s="58" t="s">
         <v>246</v>
       </c>
-      <c r="F172" s="40"/>
-      <c r="G172" s="40"/>
-      <c r="H172" s="40"/>
-      <c r="I172" s="40"/>
-      <c r="J172" s="40"/>
-      <c r="K172" s="40"/>
-      <c r="L172" s="51"/>
+      <c r="F172" s="56"/>
+      <c r="G172" s="56"/>
+      <c r="H172" s="56"/>
+      <c r="I172" s="56"/>
+      <c r="J172" s="56"/>
+      <c r="K172" s="56"/>
+      <c r="L172" s="57"/>
     </row>
     <row r="173" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E173" s="44" t="s">
+      <c r="E173" s="43" t="s">
         <v>247</v>
       </c>
-      <c r="F173" s="41"/>
-      <c r="G173" s="41"/>
-      <c r="H173" s="41"/>
-      <c r="I173" s="41"/>
-      <c r="J173" s="41"/>
-      <c r="K173" s="41"/>
-      <c r="L173" s="50"/>
+      <c r="F173" s="44"/>
+      <c r="G173" s="44"/>
+      <c r="H173" s="44"/>
+      <c r="I173" s="44"/>
+      <c r="J173" s="44"/>
+      <c r="K173" s="44"/>
+      <c r="L173" s="45"/>
     </row>
     <row r="175" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D175" s="20"/>
@@ -3937,32 +3937,32 @@
       <c r="D176" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E176" s="45" t="s">
+      <c r="E176" s="58" t="s">
         <v>250</v>
       </c>
-      <c r="F176" s="40"/>
-      <c r="G176" s="40"/>
-      <c r="H176" s="40"/>
-      <c r="I176" s="40" t="s">
+      <c r="F176" s="56"/>
+      <c r="G176" s="56"/>
+      <c r="H176" s="56"/>
+      <c r="I176" s="56" t="s">
         <v>251</v>
       </c>
-      <c r="J176" s="40"/>
-      <c r="K176" s="40"/>
-      <c r="L176" s="51"/>
+      <c r="J176" s="56"/>
+      <c r="K176" s="56"/>
+      <c r="L176" s="57"/>
     </row>
     <row r="177" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E177" s="44" t="s">
+      <c r="E177" s="43" t="s">
         <v>268</v>
       </c>
-      <c r="F177" s="41"/>
-      <c r="G177" s="41"/>
-      <c r="H177" s="41"/>
-      <c r="I177" s="41" t="s">
+      <c r="F177" s="44"/>
+      <c r="G177" s="44"/>
+      <c r="H177" s="44"/>
+      <c r="I177" s="44" t="s">
         <v>252</v>
       </c>
-      <c r="J177" s="41"/>
-      <c r="K177" s="41"/>
-      <c r="L177" s="50"/>
+      <c r="J177" s="44"/>
+      <c r="K177" s="44"/>
+      <c r="L177" s="45"/>
     </row>
     <row r="179" spans="2:13" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D179" s="18"/>
@@ -3978,28 +3978,28 @@
       <c r="D180" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E180" s="48" t="s">
+      <c r="E180" s="50" t="s">
         <v>255</v>
       </c>
-      <c r="F180" s="49"/>
-      <c r="G180" s="49"/>
-      <c r="H180" s="49"/>
-      <c r="I180" s="49"/>
-      <c r="J180" s="49"/>
-      <c r="K180" s="49"/>
-      <c r="L180" s="54"/>
+      <c r="F180" s="46"/>
+      <c r="G180" s="46"/>
+      <c r="H180" s="46"/>
+      <c r="I180" s="46"/>
+      <c r="J180" s="46"/>
+      <c r="K180" s="46"/>
+      <c r="L180" s="47"/>
     </row>
     <row r="181" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E181" s="44" t="s">
+      <c r="E181" s="43" t="s">
         <v>256</v>
       </c>
-      <c r="F181" s="41"/>
-      <c r="G181" s="41"/>
-      <c r="H181" s="41"/>
-      <c r="I181" s="41"/>
-      <c r="J181" s="41"/>
-      <c r="K181" s="41"/>
-      <c r="L181" s="50"/>
+      <c r="F181" s="44"/>
+      <c r="G181" s="44"/>
+      <c r="H181" s="44"/>
+      <c r="I181" s="44"/>
+      <c r="J181" s="44"/>
+      <c r="K181" s="44"/>
+      <c r="L181" s="45"/>
     </row>
     <row r="183" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D183" s="20"/>
@@ -4015,28 +4015,28 @@
       <c r="D184" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E184" s="55" t="s">
+      <c r="E184" s="51" t="s">
         <v>259</v>
       </c>
-      <c r="F184" s="46"/>
-      <c r="G184" s="46"/>
-      <c r="H184" s="46"/>
-      <c r="I184" s="46"/>
-      <c r="J184" s="46"/>
-      <c r="K184" s="46"/>
-      <c r="L184" s="56"/>
+      <c r="F184" s="52"/>
+      <c r="G184" s="52"/>
+      <c r="H184" s="52"/>
+      <c r="I184" s="52"/>
+      <c r="J184" s="52"/>
+      <c r="K184" s="52"/>
+      <c r="L184" s="53"/>
     </row>
     <row r="185" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E185" s="44" t="s">
+      <c r="E185" s="43" t="s">
         <v>260</v>
       </c>
-      <c r="F185" s="41"/>
-      <c r="G185" s="41"/>
-      <c r="H185" s="41"/>
-      <c r="I185" s="41"/>
-      <c r="J185" s="41"/>
-      <c r="K185" s="41"/>
-      <c r="L185" s="50"/>
+      <c r="F185" s="44"/>
+      <c r="G185" s="44"/>
+      <c r="H185" s="44"/>
+      <c r="I185" s="44"/>
+      <c r="J185" s="44"/>
+      <c r="K185" s="44"/>
+      <c r="L185" s="45"/>
     </row>
     <row r="187" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D187" s="20"/>
@@ -4052,32 +4052,32 @@
       <c r="D188" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E188" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="F188" s="43"/>
-      <c r="G188" s="40" t="s">
+      <c r="E188" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="F188" s="55"/>
+      <c r="G188" s="56" t="s">
         <v>263</v>
       </c>
-      <c r="H188" s="40"/>
-      <c r="I188" s="40"/>
-      <c r="J188" s="40"/>
-      <c r="K188" s="40"/>
-      <c r="L188" s="51"/>
+      <c r="H188" s="56"/>
+      <c r="I188" s="56"/>
+      <c r="J188" s="56"/>
+      <c r="K188" s="56"/>
+      <c r="L188" s="57"/>
     </row>
     <row r="189" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E189" s="44" t="s">
+      <c r="E189" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="F189" s="41"/>
-      <c r="G189" s="41" t="s">
+      <c r="F189" s="44"/>
+      <c r="G189" s="44" t="s">
         <v>264</v>
       </c>
-      <c r="H189" s="41"/>
-      <c r="I189" s="41"/>
-      <c r="J189" s="41"/>
-      <c r="K189" s="41"/>
-      <c r="L189" s="50"/>
+      <c r="H189" s="44"/>
+      <c r="I189" s="44"/>
+      <c r="J189" s="44"/>
+      <c r="K189" s="44"/>
+      <c r="L189" s="45"/>
     </row>
     <row r="191" spans="2:13" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D191" s="18"/>
@@ -4096,29 +4096,29 @@
       <c r="E192" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F192" s="49" t="s">
+      <c r="F192" s="46" t="s">
         <v>267</v>
       </c>
-      <c r="G192" s="49"/>
-      <c r="H192" s="49"/>
-      <c r="I192" s="49"/>
-      <c r="J192" s="49"/>
-      <c r="K192" s="49"/>
-      <c r="L192" s="54"/>
+      <c r="G192" s="46"/>
+      <c r="H192" s="46"/>
+      <c r="I192" s="46"/>
+      <c r="J192" s="46"/>
+      <c r="K192" s="46"/>
+      <c r="L192" s="47"/>
     </row>
     <row r="193" spans="2:13" x14ac:dyDescent="0.3">
       <c r="E193" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F193" s="41" t="s">
+      <c r="F193" s="44" t="s">
         <v>269</v>
       </c>
-      <c r="G193" s="41"/>
-      <c r="H193" s="41"/>
-      <c r="I193" s="41"/>
-      <c r="J193" s="41"/>
-      <c r="K193" s="41"/>
-      <c r="L193" s="50"/>
+      <c r="G193" s="44"/>
+      <c r="H193" s="44"/>
+      <c r="I193" s="44"/>
+      <c r="J193" s="44"/>
+      <c r="K193" s="44"/>
+      <c r="L193" s="45"/>
     </row>
     <row r="195" spans="2:13" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D195" s="18"/>
@@ -4134,28 +4134,28 @@
       <c r="D196" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E196" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F196" s="53"/>
-      <c r="G196" s="53"/>
-      <c r="H196" s="53"/>
-      <c r="I196" s="53"/>
-      <c r="J196" s="53"/>
-      <c r="K196" s="53"/>
-      <c r="L196" s="59"/>
+      <c r="E196" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F196" s="41"/>
+      <c r="G196" s="41"/>
+      <c r="H196" s="41"/>
+      <c r="I196" s="41"/>
+      <c r="J196" s="41"/>
+      <c r="K196" s="41"/>
+      <c r="L196" s="42"/>
     </row>
     <row r="197" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E197" s="44" t="s">
+      <c r="E197" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="F197" s="41"/>
-      <c r="G197" s="41"/>
-      <c r="H197" s="41"/>
-      <c r="I197" s="41"/>
-      <c r="J197" s="41"/>
-      <c r="K197" s="41"/>
-      <c r="L197" s="50"/>
+      <c r="F197" s="44"/>
+      <c r="G197" s="44"/>
+      <c r="H197" s="44"/>
+      <c r="I197" s="44"/>
+      <c r="J197" s="44"/>
+      <c r="K197" s="44"/>
+      <c r="L197" s="45"/>
     </row>
     <row r="199" spans="2:13" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D199" s="18"/>
@@ -4180,13 +4180,13 @@
       <c r="G200" s="23" t="s">
         <v>274</v>
       </c>
-      <c r="H200" s="57" t="s">
-        <v>20</v>
-      </c>
-      <c r="I200" s="57"/>
-      <c r="J200" s="57"/>
-      <c r="K200" s="57"/>
-      <c r="L200" s="58"/>
+      <c r="H200" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="I200" s="48"/>
+      <c r="J200" s="48"/>
+      <c r="K200" s="48"/>
+      <c r="L200" s="49"/>
     </row>
     <row r="201" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E201" s="1" t="s">
@@ -4236,28 +4236,28 @@
       <c r="D204" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E204" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F204" s="53"/>
-      <c r="G204" s="53"/>
-      <c r="H204" s="53"/>
-      <c r="I204" s="53"/>
-      <c r="J204" s="53"/>
-      <c r="K204" s="53"/>
-      <c r="L204" s="59"/>
+      <c r="E204" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F204" s="41"/>
+      <c r="G204" s="41"/>
+      <c r="H204" s="41"/>
+      <c r="I204" s="41"/>
+      <c r="J204" s="41"/>
+      <c r="K204" s="41"/>
+      <c r="L204" s="42"/>
     </row>
     <row r="205" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E205" s="44" t="s">
+      <c r="E205" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="F205" s="41"/>
-      <c r="G205" s="41"/>
-      <c r="H205" s="41"/>
-      <c r="I205" s="41"/>
-      <c r="J205" s="41"/>
-      <c r="K205" s="41"/>
-      <c r="L205" s="50"/>
+      <c r="F205" s="44"/>
+      <c r="G205" s="44"/>
+      <c r="H205" s="44"/>
+      <c r="I205" s="44"/>
+      <c r="J205" s="44"/>
+      <c r="K205" s="44"/>
+      <c r="L205" s="45"/>
     </row>
     <row r="207" spans="2:13" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D207" s="18"/>
@@ -4273,32 +4273,32 @@
       <c r="D208" s="15" t="s">
         <v>281</v>
       </c>
-      <c r="E208" s="48" t="s">
+      <c r="E208" s="50" t="s">
         <v>282</v>
       </c>
-      <c r="F208" s="49"/>
-      <c r="G208" s="53" t="s">
-        <v>20</v>
-      </c>
-      <c r="H208" s="53"/>
-      <c r="I208" s="53"/>
-      <c r="J208" s="53"/>
-      <c r="K208" s="53"/>
-      <c r="L208" s="59"/>
+      <c r="F208" s="46"/>
+      <c r="G208" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="H208" s="41"/>
+      <c r="I208" s="41"/>
+      <c r="J208" s="41"/>
+      <c r="K208" s="41"/>
+      <c r="L208" s="42"/>
     </row>
     <row r="209" spans="2:13" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E209" s="44" t="s">
+      <c r="E209" s="43" t="s">
         <v>283</v>
       </c>
-      <c r="F209" s="41"/>
-      <c r="G209" s="41" t="s">
+      <c r="F209" s="44"/>
+      <c r="G209" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="H209" s="41"/>
-      <c r="I209" s="41"/>
-      <c r="J209" s="41"/>
-      <c r="K209" s="41"/>
-      <c r="L209" s="50"/>
+      <c r="H209" s="44"/>
+      <c r="I209" s="44"/>
+      <c r="J209" s="44"/>
+      <c r="K209" s="44"/>
+      <c r="L209" s="45"/>
     </row>
     <row r="211" spans="2:13" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D211" s="18"/>
@@ -4314,28 +4314,28 @@
       <c r="D212" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E212" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F212" s="53"/>
-      <c r="G212" s="53"/>
-      <c r="H212" s="53"/>
-      <c r="I212" s="53"/>
-      <c r="J212" s="53"/>
-      <c r="K212" s="53"/>
-      <c r="L212" s="59"/>
+      <c r="E212" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F212" s="41"/>
+      <c r="G212" s="41"/>
+      <c r="H212" s="41"/>
+      <c r="I212" s="41"/>
+      <c r="J212" s="41"/>
+      <c r="K212" s="41"/>
+      <c r="L212" s="42"/>
     </row>
     <row r="213" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E213" s="44" t="s">
+      <c r="E213" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="F213" s="41"/>
-      <c r="G213" s="41"/>
-      <c r="H213" s="41"/>
-      <c r="I213" s="41"/>
-      <c r="J213" s="41"/>
-      <c r="K213" s="41"/>
-      <c r="L213" s="50"/>
+      <c r="F213" s="44"/>
+      <c r="G213" s="44"/>
+      <c r="H213" s="44"/>
+      <c r="I213" s="44"/>
+      <c r="J213" s="44"/>
+      <c r="K213" s="44"/>
+      <c r="L213" s="45"/>
     </row>
     <row r="215" spans="2:13" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D215" s="18"/>
@@ -4363,12 +4363,12 @@
       <c r="H216" s="23" t="s">
         <v>289</v>
       </c>
-      <c r="I216" s="53" t="s">
-        <v>20</v>
-      </c>
-      <c r="J216" s="53"/>
-      <c r="K216" s="53"/>
-      <c r="L216" s="59"/>
+      <c r="I216" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="J216" s="41"/>
+      <c r="K216" s="41"/>
+      <c r="L216" s="42"/>
     </row>
     <row r="217" spans="2:13" x14ac:dyDescent="0.3">
       <c r="E217" s="1" t="s">
@@ -4383,12 +4383,12 @@
       <c r="H217" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="I217" s="41" t="s">
+      <c r="I217" s="44" t="s">
         <v>290</v>
       </c>
-      <c r="J217" s="41"/>
-      <c r="K217" s="41"/>
-      <c r="L217" s="50"/>
+      <c r="J217" s="44"/>
+      <c r="K217" s="44"/>
+      <c r="L217" s="45"/>
     </row>
     <row r="219" spans="2:13" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D219" s="18"/>
@@ -4404,118 +4404,54 @@
       <c r="D220" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E220" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F220" s="53"/>
-      <c r="G220" s="53"/>
-      <c r="H220" s="53"/>
-      <c r="I220" s="53"/>
-      <c r="J220" s="53"/>
-      <c r="K220" s="53"/>
-      <c r="L220" s="59"/>
+      <c r="E220" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F220" s="41"/>
+      <c r="G220" s="41"/>
+      <c r="H220" s="41"/>
+      <c r="I220" s="41"/>
+      <c r="J220" s="41"/>
+      <c r="K220" s="41"/>
+      <c r="L220" s="42"/>
     </row>
     <row r="221" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E221" s="44" t="s">
+      <c r="E221" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="F221" s="41"/>
-      <c r="G221" s="41"/>
-      <c r="H221" s="41"/>
-      <c r="I221" s="41"/>
-      <c r="J221" s="41"/>
-      <c r="K221" s="41"/>
-      <c r="L221" s="50"/>
+      <c r="F221" s="44"/>
+      <c r="G221" s="44"/>
+      <c r="H221" s="44"/>
+      <c r="I221" s="44"/>
+      <c r="J221" s="44"/>
+      <c r="K221" s="44"/>
+      <c r="L221" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="129">
-    <mergeCell ref="E220:L220"/>
-    <mergeCell ref="E221:L221"/>
-    <mergeCell ref="E213:L213"/>
-    <mergeCell ref="E196:L196"/>
-    <mergeCell ref="E197:L197"/>
-    <mergeCell ref="E205:L205"/>
-    <mergeCell ref="G209:L209"/>
-    <mergeCell ref="E209:F209"/>
-    <mergeCell ref="G208:L208"/>
-    <mergeCell ref="I216:L216"/>
-    <mergeCell ref="E212:L212"/>
-    <mergeCell ref="I217:L217"/>
-    <mergeCell ref="F192:L192"/>
-    <mergeCell ref="F193:L193"/>
-    <mergeCell ref="H200:L200"/>
-    <mergeCell ref="E204:L204"/>
-    <mergeCell ref="E208:F208"/>
-    <mergeCell ref="E184:L184"/>
-    <mergeCell ref="E185:L185"/>
-    <mergeCell ref="E188:F188"/>
-    <mergeCell ref="E189:F189"/>
-    <mergeCell ref="G188:L188"/>
-    <mergeCell ref="G189:L189"/>
-    <mergeCell ref="E177:H177"/>
-    <mergeCell ref="I176:L176"/>
-    <mergeCell ref="I177:L177"/>
-    <mergeCell ref="E180:L180"/>
-    <mergeCell ref="E181:L181"/>
-    <mergeCell ref="E168:L168"/>
-    <mergeCell ref="E169:L169"/>
-    <mergeCell ref="E172:L172"/>
-    <mergeCell ref="E173:L173"/>
-    <mergeCell ref="E176:H176"/>
-    <mergeCell ref="E160:L160"/>
-    <mergeCell ref="E161:L161"/>
-    <mergeCell ref="F164:L164"/>
-    <mergeCell ref="F165:L165"/>
-    <mergeCell ref="E152:L152"/>
-    <mergeCell ref="E153:L153"/>
-    <mergeCell ref="F156:L156"/>
-    <mergeCell ref="F157:L157"/>
-    <mergeCell ref="E144:L144"/>
-    <mergeCell ref="E145:L145"/>
-    <mergeCell ref="E148:H148"/>
-    <mergeCell ref="I148:L148"/>
-    <mergeCell ref="E149:H149"/>
-    <mergeCell ref="I149:L149"/>
-    <mergeCell ref="E141:L141"/>
-    <mergeCell ref="E140:L140"/>
-    <mergeCell ref="F128:L128"/>
-    <mergeCell ref="F129:L129"/>
-    <mergeCell ref="E132:L132"/>
-    <mergeCell ref="E133:L133"/>
-    <mergeCell ref="F136:L136"/>
-    <mergeCell ref="F120:H120"/>
-    <mergeCell ref="J120:L120"/>
-    <mergeCell ref="F121:H121"/>
-    <mergeCell ref="J121:L121"/>
-    <mergeCell ref="E124:L124"/>
-    <mergeCell ref="E112:L112"/>
-    <mergeCell ref="E116:L116"/>
-    <mergeCell ref="E117:L117"/>
-    <mergeCell ref="E104:H104"/>
-    <mergeCell ref="I104:L104"/>
-    <mergeCell ref="E105:H105"/>
-    <mergeCell ref="I105:L105"/>
-    <mergeCell ref="E108:L108"/>
-    <mergeCell ref="F137:L137"/>
-    <mergeCell ref="E100:L100"/>
-    <mergeCell ref="E101:L101"/>
-    <mergeCell ref="E88:L88"/>
-    <mergeCell ref="E89:L89"/>
-    <mergeCell ref="E92:L92"/>
-    <mergeCell ref="F96:H96"/>
-    <mergeCell ref="I96:J96"/>
-    <mergeCell ref="K96:L96"/>
-    <mergeCell ref="E109:L109"/>
-    <mergeCell ref="E85:H85"/>
-    <mergeCell ref="I85:L85"/>
-    <mergeCell ref="E74:L74"/>
-    <mergeCell ref="E77:H77"/>
-    <mergeCell ref="I77:J77"/>
-    <mergeCell ref="K77:L77"/>
-    <mergeCell ref="K78:L78"/>
-    <mergeCell ref="K97:L97"/>
-    <mergeCell ref="I97:J97"/>
-    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="K43:L43"/>
     <mergeCell ref="E54:L54"/>
     <mergeCell ref="E55:L55"/>
     <mergeCell ref="E58:H58"/>
@@ -4535,29 +4471,93 @@
     <mergeCell ref="K59:L59"/>
     <mergeCell ref="E65:H65"/>
     <mergeCell ref="I65:L65"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="K51:L51"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="E85:H85"/>
+    <mergeCell ref="I85:L85"/>
+    <mergeCell ref="E74:L74"/>
+    <mergeCell ref="E77:H77"/>
+    <mergeCell ref="I77:J77"/>
+    <mergeCell ref="K77:L77"/>
+    <mergeCell ref="K78:L78"/>
+    <mergeCell ref="K97:L97"/>
+    <mergeCell ref="I97:J97"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="E100:L100"/>
+    <mergeCell ref="E101:L101"/>
+    <mergeCell ref="E88:L88"/>
+    <mergeCell ref="E89:L89"/>
+    <mergeCell ref="E92:L92"/>
+    <mergeCell ref="F96:H96"/>
+    <mergeCell ref="I96:J96"/>
+    <mergeCell ref="K96:L96"/>
+    <mergeCell ref="E109:L109"/>
+    <mergeCell ref="E112:L112"/>
+    <mergeCell ref="E116:L116"/>
+    <mergeCell ref="E117:L117"/>
+    <mergeCell ref="E104:H104"/>
+    <mergeCell ref="I104:L104"/>
+    <mergeCell ref="E105:H105"/>
+    <mergeCell ref="I105:L105"/>
+    <mergeCell ref="E108:L108"/>
+    <mergeCell ref="F137:L137"/>
+    <mergeCell ref="E141:L141"/>
+    <mergeCell ref="E140:L140"/>
+    <mergeCell ref="F128:L128"/>
+    <mergeCell ref="F129:L129"/>
+    <mergeCell ref="E132:L132"/>
+    <mergeCell ref="E133:L133"/>
+    <mergeCell ref="F136:L136"/>
+    <mergeCell ref="F120:H120"/>
+    <mergeCell ref="J120:L120"/>
+    <mergeCell ref="F121:H121"/>
+    <mergeCell ref="J121:L121"/>
+    <mergeCell ref="E124:L124"/>
+    <mergeCell ref="E160:L160"/>
+    <mergeCell ref="E161:L161"/>
+    <mergeCell ref="F164:L164"/>
+    <mergeCell ref="F165:L165"/>
+    <mergeCell ref="E152:L152"/>
+    <mergeCell ref="E153:L153"/>
+    <mergeCell ref="F156:L156"/>
+    <mergeCell ref="F157:L157"/>
+    <mergeCell ref="E144:L144"/>
+    <mergeCell ref="E145:L145"/>
+    <mergeCell ref="E148:H148"/>
+    <mergeCell ref="I148:L148"/>
+    <mergeCell ref="E149:H149"/>
+    <mergeCell ref="I149:L149"/>
+    <mergeCell ref="E177:H177"/>
+    <mergeCell ref="I176:L176"/>
+    <mergeCell ref="I177:L177"/>
+    <mergeCell ref="E180:L180"/>
+    <mergeCell ref="E181:L181"/>
+    <mergeCell ref="E168:L168"/>
+    <mergeCell ref="E169:L169"/>
+    <mergeCell ref="E172:L172"/>
+    <mergeCell ref="E173:L173"/>
+    <mergeCell ref="E176:H176"/>
+    <mergeCell ref="F192:L192"/>
+    <mergeCell ref="F193:L193"/>
+    <mergeCell ref="H200:L200"/>
+    <mergeCell ref="E204:L204"/>
+    <mergeCell ref="E208:F208"/>
+    <mergeCell ref="E184:L184"/>
+    <mergeCell ref="E185:L185"/>
+    <mergeCell ref="E188:F188"/>
+    <mergeCell ref="E189:F189"/>
+    <mergeCell ref="G188:L188"/>
+    <mergeCell ref="G189:L189"/>
+    <mergeCell ref="E220:L220"/>
+    <mergeCell ref="E221:L221"/>
+    <mergeCell ref="E213:L213"/>
+    <mergeCell ref="E196:L196"/>
+    <mergeCell ref="E197:L197"/>
+    <mergeCell ref="E205:L205"/>
+    <mergeCell ref="G209:L209"/>
+    <mergeCell ref="E209:F209"/>
+    <mergeCell ref="G208:L208"/>
+    <mergeCell ref="I216:L216"/>
+    <mergeCell ref="E212:L212"/>
+    <mergeCell ref="I217:L217"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8113,11 +8113,12 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="E172:E177"/>
-    <mergeCell ref="E178:E183"/>
-    <mergeCell ref="E185:E189"/>
-    <mergeCell ref="E191:E193"/>
-    <mergeCell ref="E169:E171"/>
+    <mergeCell ref="I33:I40"/>
+    <mergeCell ref="G65:G72"/>
+    <mergeCell ref="G73:G80"/>
+    <mergeCell ref="E23:E30"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="E33:E48"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="G41:G48"/>
     <mergeCell ref="G33:G40"/>
@@ -8133,12 +8134,11 @@
     <mergeCell ref="G81:G88"/>
     <mergeCell ref="G89:G96"/>
     <mergeCell ref="G97:G99"/>
-    <mergeCell ref="I33:I40"/>
-    <mergeCell ref="G65:G72"/>
-    <mergeCell ref="G73:G80"/>
-    <mergeCell ref="E23:E30"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="E33:E48"/>
+    <mergeCell ref="E172:E177"/>
+    <mergeCell ref="E178:E183"/>
+    <mergeCell ref="E185:E189"/>
+    <mergeCell ref="E191:E193"/>
+    <mergeCell ref="E169:E171"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8149,8 +8149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D315FA28-3EE9-4F24-99DB-CD202211012F}">
   <dimension ref="C5:W15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8264,11 +8264,11 @@
         <v>403</v>
       </c>
       <c r="E8">
-        <v>600</v>
+        <v>750</v>
       </c>
       <c r="F8" s="31">
         <f>E8/25</f>
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G8" t="s">
         <v>403</v>
@@ -8286,14 +8286,14 @@
       </c>
       <c r="L8" s="32">
         <f t="shared" ref="L8" si="1">(E8*1000*1000)/K8</f>
-        <v>18750000</v>
+        <v>23437500</v>
       </c>
       <c r="M8">
         <v>1</v>
       </c>
       <c r="N8" s="32">
         <f t="shared" ref="N8" si="2">(L8/M8)</f>
-        <v>18750000</v>
+        <v>23437500</v>
       </c>
     </row>
     <row r="11" spans="3:23" x14ac:dyDescent="0.3">

</xml_diff>